<commit_message>
Conferência Lista de Casamento Sige
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_Lista_Casamento_Sige_DW.xlsx
+++ b/Documentação/Planilhas/Conferencia_Lista_Casamento_Sige_DW.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="111">
   <si>
     <t>nr_id_unidade_negocio</t>
   </si>
@@ -339,6 +339,30 @@
   </si>
   <si>
     <t>????</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case 
+  when NR_STATUS_PEDIDO_LN = 2 then 'C' --Suspenso
+   when NR_STATUS_PEDIDO_LN = 5 then 'A' --Livre
+   when NR_STATUS_PEDIDO_LN = 10 then 'A' --Aprovado
+   when NR_STATUS_PEDIDO_LN = 20 and (NR_STATUS_NF_LN in (5,6)) then 'L' --Em processamento/Liquidado
+   when NR_STATUS_PEDIDO_LN = 20 and (NR_STATUS_NF_LN not in (5,6) or NR_STATUS_NF_LN is null) then 'A' --Em processamento/Aberto
+   when NR_STATUS_PEDIDO_LN = 25 then 'A' --Modificado
+   when NR_STATUS_PEDIDO_LN = 30 then 'L' --Fechado
+   when NR_STATUS_PEDIDO_LN = 35 then 'C' --Cancelado
+   when NR_STATUS_PEDIDO_LN = 40 then 'A' --Bloqueado
+   when NR_STATUS_PEDIDO_LN = 45 then 'A' --Liber.
+   when NR_STATUS_PEDIDO_LN = 50 then 'A' --Não aplicável.</t>
+  </si>
+  <si>
+    <t>Externo ao LN. Vem da Loja</t>
+  </si>
+  <si>
+    <t>Na seção "PN Receptor", pegar o código  do "Parc. De Negócios". Ir para a sessão "tccom4500m000" e informar o código na coluna "Parceiro de Negócios". Pegar a informação na coluna "Entidade Fiscal" [desprezando as "/", "-" e zeros a esquerda]</t>
+  </si>
+  <si>
+    <t>stg_lis_situacao
+Ação do usuário, (A = Aguardando, L = Liberado, V = Vale Lista)</t>
   </si>
 </sst>
 </file>
@@ -369,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +421,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,49 +482,49 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -798,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F26"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -818,125 +848,128 @@
     <col min="12" max="12" width="24.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="23.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" style="1" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="11.25" customHeight="1">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:20" ht="11.25" customHeight="1">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:20" ht="11.25" customHeight="1">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:20" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="17" t="s">
+      <c r="R5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="17" t="s">
+      <c r="S5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -956,38 +989,38 @@
       <c r="E6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="5" t="s">
         <v>65</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>30</v>
@@ -1043,10 +1076,10 @@
         <v>65</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>30</v>
@@ -1102,10 +1135,10 @@
         <v>72</v>
       </c>
       <c r="O8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>30</v>
@@ -1161,10 +1194,10 @@
         <v>65</v>
       </c>
       <c r="O9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>30</v>
@@ -1220,10 +1253,10 @@
         <v>77</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>30</v>
@@ -1275,17 +1308,17 @@
       <c r="L11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="5" t="s">
         <v>72</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>30</v>
@@ -1341,10 +1374,10 @@
         <v>85</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>43</v>
@@ -1400,10 +1433,10 @@
         <v>90</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>43</v>
@@ -1462,10 +1495,10 @@
         <v>93</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>43</v>
@@ -1521,10 +1554,10 @@
         <v>90</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>43</v>
@@ -1580,10 +1613,10 @@
         <v>41</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>30</v>
@@ -1639,10 +1672,10 @@
         <v>32</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>30</v>
@@ -1658,31 +1691,31 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="11.25" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="15" t="s">
         <v>58</v>
       </c>
       <c r="J20" s="9" t="s">
@@ -1700,156 +1733,159 @@
       <c r="N20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="O20" s="13" t="s">
+      <c r="O20" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q20" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="R20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="S20" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="P20" s="13" t="s">
+      <c r="T20" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="Q20" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="R20" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="S20" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="T20" s="13" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="5"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="5"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="5"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="Q27" s="18"/>
     </row>
     <row r="28" spans="1:20" ht="11.25" customHeight="1">
       <c r="F28" s="1" t="s">
@@ -1858,45 +1894,46 @@
       <c r="J28" s="9" t="s">
         <v>105</v>
       </c>
+      <c r="Q28" s="18"/>
     </row>
     <row r="29" spans="1:20">
       <c r="F29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="J29" s="9"/>
+      <c r="Q29" s="18"/>
     </row>
     <row r="30" spans="1:20">
       <c r="F30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J30" s="9"/>
+      <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:20">
       <c r="J31" s="9"/>
+      <c r="Q31" s="18"/>
     </row>
     <row r="32" spans="1:20">
       <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="10:10">
+      <c r="Q32" s="18"/>
+    </row>
+    <row r="33" spans="10:17">
       <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="10:10">
+      <c r="Q33" s="18"/>
+    </row>
+    <row r="34" spans="10:17">
       <c r="J34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="S20:S26"/>
-    <mergeCell ref="T20:T26"/>
-    <mergeCell ref="J28:J34"/>
-    <mergeCell ref="O20:O26"/>
-    <mergeCell ref="P20:P26"/>
-    <mergeCell ref="Q20:Q26"/>
-    <mergeCell ref="R20:R26"/>
-    <mergeCell ref="N20:N26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="Q20:Q33"/>
+    <mergeCell ref="J2:O4"/>
     <mergeCell ref="F2:I4"/>
     <mergeCell ref="B2:E4"/>
     <mergeCell ref="J20:J26"/>
-    <mergeCell ref="J2:N4"/>
     <mergeCell ref="G20:G26"/>
     <mergeCell ref="H20:H26"/>
     <mergeCell ref="I20:I26"/>
@@ -1907,8 +1944,13 @@
     <mergeCell ref="C20:C26"/>
     <mergeCell ref="E20:E26"/>
     <mergeCell ref="D20:D26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="S20:S26"/>
+    <mergeCell ref="T20:T26"/>
+    <mergeCell ref="J28:J34"/>
+    <mergeCell ref="P20:P26"/>
+    <mergeCell ref="O20:O26"/>
+    <mergeCell ref="R20:R26"/>
+    <mergeCell ref="N20:N26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>